<commit_message>
settings(protocol) test case added
</commit_message>
<xml_diff>
--- a/apps/features/backlog/desktop/windows/get support/get_support.xlsx
+++ b/apps/features/backlog/desktop/windows/get support/get_support.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\apps\features\backlog\desktop\windows\get support\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91891EF9-995E-4303-A479-FA411254F27F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9400A0F5-4779-4CCE-ACD7-8AC8BFE65354}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,10 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
-  <si>
-    <t xml:space="preserve">Jira Task No: 1419 </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -69,9 +66,6 @@
   </si>
   <si>
     <t>TC_SYM_GSF_004</t>
-  </si>
-  <si>
-    <t>Support Features Accessibility</t>
   </si>
   <si>
     <t>Verify E-mail Support</t>
@@ -118,13 +112,6 @@
 5. Navigate to the "Support" section.
 6. Review the FAQ section for common queries and issues.
 7. Confirm that the answers provided are relevant, comprehensive and clear</t>
-  </si>
-  <si>
-    <t>1. Go to Playstore and install SymlexVPN in the desktop.
-2. Open the installed SymlexVPN Application.
-3. Login with proper credentials.
-4. Go to menubar
-5. Navigate to the "Support" section.</t>
   </si>
   <si>
     <t>Ensure that all support features (WhatsApp, email,
@@ -374,21 +361,37 @@
 or connection issues during user interactions</t>
   </si>
   <si>
-    <t>check cross-browser compatibility for support 
-page</t>
+    <t>the "Support Page" functions consistently across 
+various web browsers, ensuring a seamless user 
+experience</t>
+  </si>
+  <si>
+    <t>check cross-browser compatibility for FAQ</t>
   </si>
   <si>
     <t>1. Go to Playstore and install SymlexVPN in the desktop.
 2. Open the installed SymlexVPN Application.
 3. Login with proper credentials.
 4. Go to menubar
-5. try to check cross-browser compatibility for support 
-page</t>
+5. try to check check cross-browser compatibility for FAQ</t>
   </si>
   <si>
-    <t>the "Support Page" functions consistently across 
-various web browsers, ensuring a seamless user 
-experience</t>
+    <t>Test Scenario : Get Support page for desktop windows</t>
+  </si>
+  <si>
+    <t>check support Features Accessibility</t>
+  </si>
+  <si>
+    <t>1. Go to Playstore and install SymlexVPN in the desktop.
+2. Open the installed SymlexVPN Application.
+3. Login with proper credentials.
+4. Go to menubar
+5. Navigate to the "Support" section.
+6. check support features accessibility</t>
+  </si>
+  <si>
+    <t>1. app need to be installed
+2. login with credentials</t>
   </si>
 </sst>
 </file>
@@ -647,7 +650,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -719,14 +722,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -741,6 +736,17 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1540,8 +1546,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="3" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1557,15 +1563,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
-        <v>0</v>
+      <c r="A1" s="30" t="s">
+        <v>84</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="27"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="32"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1587,13 +1593,13 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="35"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
@@ -1616,25 +1622,25 @@
     </row>
     <row r="3" spans="1:26" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="E3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1658,23 +1664,23 @@
     </row>
     <row r="4" spans="1:26" ht="143.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="11"/>
       <c r="C4" s="11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -1698,20 +1704,20 @@
     </row>
     <row r="5" spans="1:26" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="4"/>
@@ -1736,20 +1742,22 @@
     </row>
     <row r="6" spans="1:26" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
-      <c r="B6" s="9"/>
+      <c r="B6" s="36" t="s">
+        <v>87</v>
+      </c>
       <c r="C6" s="17" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="4"/>
@@ -1772,22 +1780,22 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="4"/>
     </row>
-    <row r="7" spans="1:26" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="17" t="s">
-        <v>14</v>
+      <c r="C7" s="27" t="s">
+        <v>85</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>24</v>
+      <c r="D7" s="27" t="s">
+        <v>86</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="4"/>
@@ -1812,17 +1820,17 @@
     </row>
     <row r="8" spans="1:26" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="19" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
@@ -1848,17 +1856,17 @@
     </row>
     <row r="9" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="24"/>
       <c r="C9" s="24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" s="24" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F9" s="24"/>
       <c r="G9" s="24"/>
@@ -1884,17 +1892,17 @@
     </row>
     <row r="10" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="23" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B10" s="21"/>
       <c r="C10" s="21" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F10" s="21"/>
       <c r="G10" s="21"/>
@@ -1920,19 +1928,19 @@
     </row>
     <row r="11" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="23" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F11" s="22"/>
       <c r="G11" s="22"/>
@@ -1958,19 +1966,19 @@
     </row>
     <row r="12" spans="1:26" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="23" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F12" s="22"/>
       <c r="G12" s="22"/>
@@ -1996,19 +2004,19 @@
     </row>
     <row r="13" spans="1:26" ht="92.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E13" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F13" s="22"/>
       <c r="G13" s="22"/>
@@ -2034,19 +2042,19 @@
     </row>
     <row r="14" spans="1:26" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C14" s="21" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E14" s="22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
@@ -2072,19 +2080,19 @@
     </row>
     <row r="15" spans="1:26" ht="95.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C15" s="21" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F15" s="22"/>
       <c r="G15" s="22"/>
@@ -2109,20 +2117,20 @@
       <c r="Z15" s="1"/>
     </row>
     <row r="16" spans="1:26" ht="93" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="31" t="s">
-        <v>40</v>
+      <c r="A16" s="25" t="s">
+        <v>37</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>50</v>
+      <c r="B16" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="C16" s="34" t="s">
-        <v>59</v>
+      <c r="C16" s="28" t="s">
+        <v>56</v>
       </c>
-      <c r="D16" s="33" t="s">
-        <v>61</v>
+      <c r="D16" s="27" t="s">
+        <v>58</v>
       </c>
-      <c r="E16" s="35" t="s">
-        <v>60</v>
+      <c r="E16" s="29" t="s">
+        <v>57</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2147,20 +2155,20 @@
       <c r="Z16" s="1"/>
     </row>
     <row r="17" spans="1:26" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="31" t="s">
-        <v>41</v>
+      <c r="A17" s="25" t="s">
+        <v>38</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>50</v>
+      <c r="B17" s="26" t="s">
+        <v>47</v>
       </c>
-      <c r="C17" s="34" t="s">
-        <v>62</v>
+      <c r="C17" s="28" t="s">
+        <v>59</v>
       </c>
-      <c r="D17" s="33" t="s">
-        <v>64</v>
+      <c r="D17" s="27" t="s">
+        <v>61</v>
       </c>
-      <c r="E17" s="35" t="s">
-        <v>63</v>
+      <c r="E17" s="29" t="s">
+        <v>60</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -2185,18 +2193,18 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="31" t="s">
-        <v>42</v>
+      <c r="A18" s="25" t="s">
+        <v>39</v>
       </c>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34" t="s">
-        <v>65</v>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28" t="s">
+        <v>62</v>
       </c>
-      <c r="D18" s="33" t="s">
-        <v>66</v>
+      <c r="D18" s="27" t="s">
+        <v>63</v>
       </c>
-      <c r="E18" s="35" t="s">
-        <v>67</v>
+      <c r="E18" s="29" t="s">
+        <v>64</v>
       </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -2221,18 +2229,18 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="31" t="s">
-        <v>43</v>
+      <c r="A19" s="25" t="s">
+        <v>40</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34" t="s">
-        <v>68</v>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28" t="s">
+        <v>65</v>
       </c>
-      <c r="D19" s="33" t="s">
-        <v>69</v>
+      <c r="D19" s="27" t="s">
+        <v>66</v>
       </c>
-      <c r="E19" s="35" t="s">
-        <v>70</v>
+      <c r="E19" s="29" t="s">
+        <v>67</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
@@ -2257,20 +2265,20 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="31" t="s">
-        <v>71</v>
+      <c r="A20" s="25" t="s">
+        <v>68</v>
       </c>
-      <c r="B20" s="34" t="s">
-        <v>50</v>
+      <c r="B20" s="28" t="s">
+        <v>47</v>
       </c>
-      <c r="C20" s="34" t="s">
-        <v>75</v>
+      <c r="C20" s="28" t="s">
+        <v>72</v>
       </c>
-      <c r="D20" s="33" t="s">
-        <v>76</v>
+      <c r="D20" s="27" t="s">
+        <v>73</v>
       </c>
-      <c r="E20" s="35" t="s">
-        <v>77</v>
+      <c r="E20" s="29" t="s">
+        <v>74</v>
       </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
@@ -2295,20 +2303,20 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="86.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="31" t="s">
-        <v>72</v>
+      <c r="A21" s="25" t="s">
+        <v>69</v>
       </c>
-      <c r="B21" s="34" t="s">
-        <v>50</v>
+      <c r="B21" s="28" t="s">
+        <v>47</v>
       </c>
-      <c r="C21" s="34" t="s">
-        <v>80</v>
+      <c r="C21" s="28" t="s">
+        <v>77</v>
       </c>
-      <c r="D21" s="33" t="s">
-        <v>79</v>
+      <c r="D21" s="27" t="s">
+        <v>76</v>
       </c>
-      <c r="E21" s="35" t="s">
-        <v>78</v>
+      <c r="E21" s="29" t="s">
+        <v>75</v>
       </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
@@ -2333,20 +2341,20 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="83.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="31" t="s">
-        <v>73</v>
+      <c r="A22" s="25" t="s">
+        <v>70</v>
       </c>
-      <c r="B22" s="34" t="s">
-        <v>50</v>
+      <c r="B22" s="28" t="s">
+        <v>47</v>
       </c>
-      <c r="C22" s="34" t="s">
-        <v>81</v>
+      <c r="C22" s="28" t="s">
+        <v>78</v>
       </c>
-      <c r="D22" s="33" t="s">
-        <v>82</v>
+      <c r="D22" s="27" t="s">
+        <v>79</v>
       </c>
-      <c r="E22" s="35" t="s">
-        <v>83</v>
+      <c r="E22" s="29" t="s">
+        <v>80</v>
       </c>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
@@ -2371,20 +2379,20 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" ht="108.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="31" t="s">
-        <v>74</v>
+      <c r="A23" s="25" t="s">
+        <v>71</v>
       </c>
-      <c r="B23" s="34" t="s">
-        <v>50</v>
+      <c r="B23" s="28" t="s">
+        <v>47</v>
       </c>
-      <c r="C23" s="35" t="s">
-        <v>84</v>
+      <c r="C23" s="29" t="s">
+        <v>82</v>
       </c>
-      <c r="D23" s="33" t="s">
-        <v>85</v>
+      <c r="D23" s="27" t="s">
+        <v>83</v>
       </c>
-      <c r="E23" s="35" t="s">
-        <v>86</v>
+      <c r="E23" s="29" t="s">
+        <v>81</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>

</xml_diff>